<commit_message>
PROS-6202 - CCRU - Hypermarket template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Hypermarket PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Hypermarket PoS 2018.xlsx
@@ -13,49 +13,50 @@
     <sheet name="Alcomarket" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AR$313</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Hypermarket!$A$1:$AS$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1414,7 +1415,7 @@
     <t xml:space="preserve">Moya Semya - Citrus Mix - 1.93L, Moya Semya - Citrus Mix - 2L</t>
   </si>
   <si>
-    <t xml:space="preserve">4650075421376, 4650075421376</t>
+    <t xml:space="preserve">4650075421376, 4650075420034</t>
   </si>
   <si>
     <t xml:space="preserve">Moya Semya - Apricot-Peach - 1.93L</t>
@@ -3772,16 +3773,16 @@
   <dimension ref="A1:AR313"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G129" activeCellId="0" sqref="G129"/>
+      <selection pane="bottomLeft" activeCell="L130" activeCellId="0" sqref="L130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="45.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="14.7125506072875"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="15.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="33.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30893,7 +30894,7 @@
       <c r="AR313" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS313"/>
+  <autoFilter ref="A1:AR313"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>